<commit_message>
Add validate to import employee info
</commit_message>
<xml_diff>
--- a/ESMS.BackendAPI/Excel/EmpTemplate.xlsx
+++ b/ESMS.BackendAPI/Excel/EmpTemplate.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Capstone\Backend3\ESMS.BackendAPI\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BaoNG" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" refMode="R1C1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -63,11 +63,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0000000000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,11 +82,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="MS PGothic"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="20"/>
       <color rgb="FF000000"/>
@@ -139,6 +133,25 @@
       <color rgb="FFFF0000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Var(--ff-mono)"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF454545"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -161,7 +174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -194,162 +207,109 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="hair">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -358,30 +318,37 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
@@ -389,215 +356,136 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="15" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -611,6 +499,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>83105</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1628775</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>666750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2045255" y="219077"/>
+          <a:ext cx="1545670" cy="638173"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -876,217 +813,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.7109375" customWidth="1"/>
     <col min="4" max="4" width="28.140625" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="6" max="6" width="37.7109375" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
     <col min="7" max="7" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3"/>
-      <c r="B1" s="6"/>
+      <c r="B1" s="5"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="30"/>
+      <c r="G1" s="14"/>
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" ht="54.75" customHeight="1">
-      <c r="A2" s="14"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="34" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3"/>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="25"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="20" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="26"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="44"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3"/>
-      <c r="B6" s="5"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="1"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3"/>
-      <c r="B7" s="6"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3"/>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="31"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3"/>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="20" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="16"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="17"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="17"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="17"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="17"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="17"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="17"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="29"/>
       <c r="E16" s="29"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="17"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3"/>
-      <c r="B18" s="6"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1096,7 +1033,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="3"/>
-      <c r="B19" s="6"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1106,17 +1043,48 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="3"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="15"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
+    <row r="21" spans="1:8">
+      <c r="C21" s="17"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="C23" s="16"/>
+    </row>
   </sheetData>
+  <dataConsolidate/>
   <mergeCells count="4">
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
   </mergeCells>
+  <dataValidations count="6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F1048576">
+      <formula1>"'=and(len(F10)=10,isnumber((f10))'"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
+      <formula1>AND(LEN(B10)&gt;=3,LEN(B10)&lt;=50,IF(B10="",TRUE,IF(ISERROR(SUMPRODUCT(SEARCH(MID(B10,ROW(INDIRECT("1:"&amp;LEN(B10))),1),"qazwsxedcrfvtgbyhnujmikolpàáảãạăằắẳẵặâầấẩẫậèéẻẽẹêềếểễệìíỉĩịòóỏõọôồốổỗộơờớởỡợùúủũụưừứửữựỳýỷỹỵ"))),FALSE,TRUE)))</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+      <formula1>1</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10">
+      <formula1>AND(LEN(D10)&gt;=10,LEN(D10)&lt;=12,IF(D10="",TRUE,IF(ISERROR(SUMPRODUCT(SEARCH(MID(D10,ROW(INDIRECT("1:"&amp;LEN(B10))),1),"0123456789"))),FALSE,TRUE)))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10">
+      <formula1>AND(IFERROR(FIND(".",E10),FALSE),IFERROR(FIND(".",E10,FIND("@",E10)),FALSE))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10">
+      <formula1>AND(LEFT(F10,1)="0",MID(F10,2,1)&lt;&gt;"0",LEN(F10)=10,IF(F10="",TRUE,IF(ISERROR(SUMPRODUCT(SEARCH(MID(F10,ROW(INDIRECT("1:"&amp;LEN(F10))),1),"0123456789"))),FALSE,TRUE)))</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add creator name and issue date to template
</commit_message>
<xml_diff>
--- a/ESMS.BackendAPI/Excel/EmpTemplate.xlsx
+++ b/ESMS.BackendAPI/Excel/EmpTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Capstone\Backend3\ESMS.BackendAPI\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="BaoNG" sheetId="1" r:id="rId1"/>
@@ -64,9 +64,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0000000000"/>
+    <numFmt numFmtId="164" formatCode="0000000000"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +152,12 @@
       <color rgb="FF454545"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -442,7 +448,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
@@ -459,29 +465,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -816,7 +822,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E4" sqref="E4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -841,12 +847,12 @@
     </row>
     <row r="2" spans="1:8" ht="54.75" customHeight="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="37"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="40"/>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="39"/>
+      <c r="E2" s="37"/>
       <c r="F2" s="38"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>

</xml_diff>